<commit_message>
added anser to question in M4 PS1
</commit_message>
<xml_diff>
--- a/M4/exercises/discrete_vs_compounded.xlsx
+++ b/M4/exercises/discrete_vs_compounded.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14680" yWindow="120" windowWidth="13860" windowHeight="15100" activeTab="1"/>
+    <workbookView xWindow="3580" yWindow="120" windowWidth="24960" windowHeight="15720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Q2" sheetId="1" r:id="rId1"/>
     <sheet name="Q4" sheetId="5" r:id="rId2"/>
+    <sheet name="Q5" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Q2'!$D$1:$F$202</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Principal</t>
   </si>
@@ -80,6 +81,15 @@
   </si>
   <si>
     <t>Wtd Time^2</t>
+  </si>
+  <si>
+    <t>Time to maturity</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Fwd Rate</t>
   </si>
 </sst>
 </file>
@@ -3931,11 +3941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109094152"/>
-        <c:axId val="2109095768"/>
+        <c:axId val="2124893304"/>
+        <c:axId val="2124841608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109094152"/>
+        <c:axId val="2124893304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3945,12 +3955,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109095768"/>
+        <c:crossAx val="2124841608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2109095768"/>
+        <c:axId val="2124841608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3961,7 +3971,205 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109094152"/>
+        <c:crossAx val="2124893304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q5'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>YTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Q5'!$A:$A</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Time to maturity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q5'!$C:$C</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0725706928348354</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0992254693619191</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.100368364261307</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q5'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fwd Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Q5'!$A:$A</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Time to maturity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q5'!$D:$D</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0725706928348354</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.125880245889003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.102654154060083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2127250792"/>
+        <c:axId val="2126740072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2127250792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2126740072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2126740072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2127250792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3977,7 +4185,165 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q5'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>YTM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q5'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0725706928348354</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0992254693619191</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.100368364261307</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q5'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fwd Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q5'!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0725706928348354</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125880245889003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.102654154060083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2107024136"/>
+        <c:axId val="2127296584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2107024136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2127296584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2127296584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2107024136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4010,6 +4376,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>944880</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>345440</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>157480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>40640</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>157480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8593,7 +9024,7 @@
         <v>96</v>
       </c>
       <c r="E194">
-        <f t="shared" ref="E194:E257" si="15">P*(1+rate/m)^(D194*m)</f>
+        <f t="shared" ref="E194:E202" si="15">P*(1+rate/m)^(D194*m)</f>
         <v>661.97663019008769</v>
       </c>
       <c r="F194">
@@ -8878,7 +9309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -9100,4 +9531,90 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.93</v>
+      </c>
+      <c r="C2">
+        <f>-LN(B2)/A2</f>
+        <v>7.2570692834835374E-2</v>
+      </c>
+      <c r="D2">
+        <f>C2</f>
+        <v>7.2570692834835374E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.82</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="0">-LN(B3)/A3</f>
+        <v>9.9225469361919158E-2</v>
+      </c>
+      <c r="D3">
+        <f>(C3*A3-C2*A2)/(A3-A2)</f>
+        <v>0.12588024588900293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.74</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.1003683642613072</v>
+      </c>
+      <c r="D4">
+        <f>(C4*A4-C3*A3)/(A4-A3)</f>
+        <v>0.1026541540600833</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>